<commit_message>
updates to LME analysis
Write up highlighted weaknesses in analysis!
</commit_message>
<xml_diff>
--- a/Ch_7_Sentence_Modes/Excel/Mode OR Nuc PA Phonetic Models.xlsx
+++ b/Ch_7_Sentence_Modes/Excel/Mode OR Nuc PA Phonetic Models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7439359B-8861-4F8A-8289-D92A2C18B550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD7DA39-FE3A-4204-8A2B-7FCE3D755A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="4" activeTab="4" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
   </bookViews>
   <sheets>
     <sheet name="B0 Mode" sheetId="8" r:id="rId1"/>
@@ -58,12 +58,6 @@
     <externalReference r:id="rId41"/>
     <externalReference r:id="rId42"/>
     <externalReference r:id="rId43"/>
-    <externalReference r:id="rId44"/>
-    <externalReference r:id="rId45"/>
-    <externalReference r:id="rId46"/>
-    <externalReference r:id="rId47"/>
-    <externalReference r:id="rId48"/>
-    <externalReference r:id="rId49"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'B0 Mode'!$A$1:$AM$10</definedName>
@@ -91,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="73">
   <si>
     <t>Predictors</t>
   </si>
@@ -484,6 +478,9 @@
   </si>
   <si>
     <t>p.adj.</t>
+  </si>
+  <si>
+    <t>p&lt;0.001</t>
   </si>
 </sst>
 </file>
@@ -2169,225 +2166,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="146">
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD95F02"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFD95F02"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD95F02"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFD95F02"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD95F02"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD95F02"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFD95F02"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFD95F02"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF1B9E77"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -5152,6 +4930,225 @@
         <i val="0"/>
         <color rgb="FF00B050"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD95F02"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFD95F02"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF1B9E77"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <font>
@@ -14481,7 +14478,7 @@
             <v>0.41470000000000001</v>
           </cell>
           <cell r="J2">
-            <v>0.48899999999999999</v>
+            <v>0.48470000000000002</v>
           </cell>
         </row>
         <row r="3">
@@ -14507,7 +14504,7 @@
             <v>0.82399999999999995</v>
           </cell>
           <cell r="J3">
-            <v>0.89959999999999996</v>
+            <v>0.89349999999999996</v>
           </cell>
         </row>
         <row r="4">
@@ -14533,7 +14530,7 @@
             <v>2.3999999999999998E-3</v>
           </cell>
           <cell r="J4">
-            <v>3.8E-3</v>
+            <v>4.0000000000000001E-3</v>
           </cell>
           <cell r="K4" t="str">
             <v>p&lt;0.01</v>
@@ -14562,7 +14559,7 @@
             <v>0.69210000000000005</v>
           </cell>
           <cell r="J5">
-            <v>0.76219999999999999</v>
+            <v>0.75649999999999995</v>
           </cell>
         </row>
         <row r="6">
@@ -14588,7 +14585,7 @@
             <v>1.2200000000000001E-2</v>
           </cell>
           <cell r="J6">
-            <v>1.6899999999999998E-2</v>
+            <v>1.7399999999999999E-2</v>
           </cell>
           <cell r="K6" t="str">
             <v>p&lt;0.05</v>
@@ -14617,7 +14614,7 @@
             <v>2.04E-4</v>
           </cell>
           <cell r="J7">
-            <v>4.4299999999999998E-4</v>
+            <v>4.5899999999999999E-4</v>
           </cell>
           <cell r="K7" t="str">
             <v>p&lt;0.001</v>
@@ -17355,162 +17352,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink37.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="l_f0_b0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="B2">
-            <v>87.427999999999997</v>
-          </cell>
-          <cell r="C2">
-            <v>1.07</v>
-          </cell>
-          <cell r="D2">
-            <v>85.331000000000003</v>
-          </cell>
-          <cell r="E2">
-            <v>89.525999999999996</v>
-          </cell>
-          <cell r="F2">
-            <v>81.691000000000003</v>
-          </cell>
-          <cell r="G2">
-            <v>10.130000000000001</v>
-          </cell>
-          <cell r="H2">
-            <v>1.2761E-15</v>
-          </cell>
-          <cell r="I2">
-            <v>2.04E-14</v>
-          </cell>
-          <cell r="J2" t="str">
-            <v>p&lt;0.001</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>87.581999999999994</v>
-          </cell>
-          <cell r="C3">
-            <v>1.143</v>
-          </cell>
-          <cell r="D3">
-            <v>85.340999999999994</v>
-          </cell>
-          <cell r="E3">
-            <v>89.822999999999993</v>
-          </cell>
-          <cell r="F3">
-            <v>76.599999999999994</v>
-          </cell>
-          <cell r="G3">
-            <v>11.21</v>
-          </cell>
-          <cell r="H3">
-            <v>1.3445E-16</v>
-          </cell>
-          <cell r="I3">
-            <v>2.1499999999999998E-15</v>
-          </cell>
-          <cell r="J3" t="str">
-            <v>p&lt;0.001</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>89.210999999999999</v>
-          </cell>
-          <cell r="C4">
-            <v>1.1830000000000001</v>
-          </cell>
-          <cell r="D4">
-            <v>86.893000000000001</v>
-          </cell>
-          <cell r="E4">
-            <v>91.53</v>
-          </cell>
-          <cell r="F4">
-            <v>75.412000000000006</v>
-          </cell>
-          <cell r="G4">
-            <v>9.26</v>
-          </cell>
-          <cell r="H4">
-            <v>3.1473E-14</v>
-          </cell>
-          <cell r="I4">
-            <v>5.0399999999999997E-13</v>
-          </cell>
-          <cell r="J4" t="str">
-            <v>p&lt;0.001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>90.358999999999995</v>
-          </cell>
-          <cell r="C5">
-            <v>1.395</v>
-          </cell>
-          <cell r="D5">
-            <v>87.625</v>
-          </cell>
-          <cell r="E5">
-            <v>93.093000000000004</v>
-          </cell>
-          <cell r="F5">
-            <v>64.771000000000001</v>
-          </cell>
-          <cell r="G5">
-            <v>10.92</v>
-          </cell>
-          <cell r="H5">
-            <v>1.8184000000000001E-15</v>
-          </cell>
-          <cell r="I5">
-            <v>2.9099999999999997E-14</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>p&lt;0.001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink38.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="h_f0_b0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink39.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="f0_exc_b0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -17530,45 +17371,6 @@
           </cell>
         </row>
       </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink40.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="l_t_b0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink41.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="h_t_b0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink42.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="lh_slope_b0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -17605,7 +17407,7 @@
             <v>4.9800000000000003E-8</v>
           </cell>
           <cell r="I2">
-            <v>1.5800000000000001E-7</v>
+            <v>1.68E-7</v>
           </cell>
           <cell r="J2" t="str">
             <v>p&lt;0.0001</v>
@@ -17634,7 +17436,7 @@
             <v>7.6700000000000005E-8</v>
           </cell>
           <cell r="I3">
-            <v>2.34E-7</v>
+            <v>2.4699999999999998E-7</v>
           </cell>
           <cell r="J3" t="str">
             <v>p&lt;0.0001</v>
@@ -17663,7 +17465,7 @@
             <v>3.99E-8</v>
           </cell>
           <cell r="I4">
-            <v>1.2800000000000001E-7</v>
+            <v>1.36E-7</v>
           </cell>
           <cell r="J4" t="str">
             <v>p&lt;0.0001</v>
@@ -17692,7 +17494,7 @@
             <v>3.2000000000000002E-8</v>
           </cell>
           <cell r="I5">
-            <v>1.05E-7</v>
+            <v>1.12E-7</v>
           </cell>
           <cell r="J5" t="str">
             <v>p&lt;0.0001</v>
@@ -18025,22 +17827,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3980010-2201-43EF-9941-5D34E4A5CF0F}" name="Table1" displayName="Table1" ref="M2:W10" totalsRowShown="0" headerRowDxfId="130" dataDxfId="128" headerRowBorderDxfId="129" tableBorderDxfId="127" totalsRowBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3980010-2201-43EF-9941-5D34E4A5CF0F}" name="Table1" displayName="Table1" ref="M2:W10" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94" tableBorderDxfId="92" totalsRowBorderDxfId="91">
   <autoFilter ref="M2:W10" xr:uid="{D3980010-2201-43EF-9941-5D34E4A5CF0F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{48EA7560-AFDA-4976-872C-A62413C27C30}" name="Predictors" dataDxfId="125">
+    <tableColumn id="1" xr3:uid="{48EA7560-AFDA-4976-872C-A62413C27C30}" name="Predictors" dataDxfId="90">
       <calculatedColumnFormula>Table5[[#This Row],[Predictors]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B74BAF5A-A8B1-41AC-AA5C-9C7F4D3C00F5}" name="estimate" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{692BDF21-5E37-4774-A232-65FEAC4EF62A}" name="std.error" dataDxfId="123"/>
-    <tableColumn id="6" xr3:uid="{25F0D2CD-4553-4F0F-A005-7B069A4DF146}" name="2.5% CI" dataDxfId="122"/>
-    <tableColumn id="5" xr3:uid="{5C65DEBD-594B-4030-A893-0F5416AC8463}" name="97.5% CI" dataDxfId="121"/>
-    <tableColumn id="9" xr3:uid="{FB617D51-EF00-47A5-9763-9BB9A4CEB416}" name="t.value" dataDxfId="120"/>
-    <tableColumn id="12" xr3:uid="{BCFF8561-1231-4432-9628-4F22307BB92D}" name="df" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{1C749EC2-7DA5-4835-AAB4-29FE5E444F42}" name="p.value" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{0603EEF6-D289-414E-9A6C-56120260E64A}" name="p.adj." dataDxfId="117"/>
-    <tableColumn id="10" xr3:uid="{B6EB825D-CAC4-470B-89BB-4D3BB4C21701}" name="signif. " dataDxfId="116"/>
-    <tableColumn id="8" xr3:uid="{C1996589-8716-4257-9BC3-42E65902C402}" name="|CI-delta|" dataDxfId="115">
+    <tableColumn id="2" xr3:uid="{B74BAF5A-A8B1-41AC-AA5C-9C7F4D3C00F5}" name="estimate" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{692BDF21-5E37-4774-A232-65FEAC4EF62A}" name="std.error" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{25F0D2CD-4553-4F0F-A005-7B069A4DF146}" name="2.5% CI" dataDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{5C65DEBD-594B-4030-A893-0F5416AC8463}" name="97.5% CI" dataDxfId="86"/>
+    <tableColumn id="9" xr3:uid="{FB617D51-EF00-47A5-9763-9BB9A4CEB416}" name="t.value" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{BCFF8561-1231-4432-9628-4F22307BB92D}" name="df" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{1C749EC2-7DA5-4835-AAB4-29FE5E444F42}" name="p.value" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{0603EEF6-D289-414E-9A6C-56120260E64A}" name="p.adj." dataDxfId="82"/>
+    <tableColumn id="10" xr3:uid="{B6EB825D-CAC4-470B-89BB-4D3BB4C21701}" name="signif. " dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{C1996589-8716-4257-9BC3-42E65902C402}" name="|CI-delta|" dataDxfId="80">
       <calculatedColumnFormula>N3-P3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18049,40 +17851,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE40A492-BBA9-4876-8724-BC64B3994271}" name="Table3" displayName="Table3" ref="M13:W21" totalsRowShown="0" headerRowDxfId="114" dataDxfId="112" headerRowBorderDxfId="113" tableBorderDxfId="111" totalsRowBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE40A492-BBA9-4876-8724-BC64B3994271}" name="Table3" displayName="Table3" ref="M13:W21" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <autoFilter ref="M13:W21" xr:uid="{DE40A492-BBA9-4876-8724-BC64B3994271}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E34199D2-D5CB-45DC-96B2-AAECCF32344B}" name="Predictors" dataDxfId="109">
+    <tableColumn id="1" xr3:uid="{E34199D2-D5CB-45DC-96B2-AAECCF32344B}" name="Predictors" dataDxfId="74">
       <calculatedColumnFormula>A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{BF536D58-8825-421A-A286-3483AB4A0DBA}" name="estimate" dataDxfId="108">
-      <calculatedColumnFormula>[38]h_f0_b0!B2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{2B81C313-1E48-4C7B-A992-DEE392DF89F2}" name="std.error" dataDxfId="107">
-      <calculatedColumnFormula>[38]h_f0_b0!C2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{51E253F3-5545-4607-87E2-3713F0C79ED0}" name="2.5% CI" dataDxfId="106">
-      <calculatedColumnFormula>[38]h_f0_b0!D2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{39D9684C-88E4-42B1-822E-8BF560658BA3}" name="97.5% CI" dataDxfId="105">
-      <calculatedColumnFormula>[38]h_f0_b0!E2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{8C5A2141-4E8D-4B51-91E2-E311E1CE8B0F}" name="t.value" dataDxfId="104">
-      <calculatedColumnFormula>[38]h_f0_b0!F2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{B4DE621E-08D1-4FCC-B6B4-06AD6DA726A0}" name="df" dataDxfId="103">
-      <calculatedColumnFormula>[38]h_f0_b0!G2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{5CF7E86F-7A72-45EB-8BFA-3C614A5C05E4}" name="p.value" dataDxfId="102">
-      <calculatedColumnFormula>[38]h_f0_b0!H2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{2C1E6FA3-F11F-4631-B0BB-23F7331F52BE}" name="p.adj." dataDxfId="101">
-      <calculatedColumnFormula>[38]h_f0_b0!I2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{0BFD4196-49FF-4FB8-BB68-47C4305BC767}" name="signif. " dataDxfId="100">
-      <calculatedColumnFormula>[38]h_f0_b0!J2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{91174BE1-7871-4821-9200-FC6E6061BBAE}" name="|CI-delta|" dataDxfId="99">
+    <tableColumn id="2" xr3:uid="{BF536D58-8825-421A-A286-3483AB4A0DBA}" name="estimate" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{2B81C313-1E48-4C7B-A992-DEE392DF89F2}" name="std.error" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{51E253F3-5545-4607-87E2-3713F0C79ED0}" name="2.5% CI" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{39D9684C-88E4-42B1-822E-8BF560658BA3}" name="97.5% CI" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{8C5A2141-4E8D-4B51-91E2-E311E1CE8B0F}" name="t.value" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{B4DE621E-08D1-4FCC-B6B4-06AD6DA726A0}" name="df" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{5CF7E86F-7A72-45EB-8BFA-3C614A5C05E4}" name="p.value" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{2C1E6FA3-F11F-4631-B0BB-23F7331F52BE}" name="p.adj." dataDxfId="66"/>
+    <tableColumn id="10" xr3:uid="{0BFD4196-49FF-4FB8-BB68-47C4305BC767}" name="signif. " dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{91174BE1-7871-4821-9200-FC6E6061BBAE}" name="|CI-delta|" dataDxfId="64">
       <calculatedColumnFormula>N14-P14</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18091,40 +17875,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BDDC793-1E7A-4B5C-BD08-84F047AC5B6B}" name="Table4" displayName="Table4" ref="Y2:AI10" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BDDC793-1E7A-4B5C-BD08-84F047AC5B6B}" name="Table4" displayName="Table4" ref="Y2:AI10" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="Y2:AI10" xr:uid="{6BDDC793-1E7A-4B5C-BD08-84F047AC5B6B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{82A813F0-7850-4939-B6AE-4F49D1DC217D}" name="Predictors" dataDxfId="93">
+    <tableColumn id="1" xr3:uid="{82A813F0-7850-4939-B6AE-4F49D1DC217D}" name="Predictors" dataDxfId="58">
       <calculatedColumnFormula>Table5[[#This Row],[Predictors]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{352EAC9D-A02A-4CE8-AF89-3ED3FCB5A979}" name="estimate" dataDxfId="92">
-      <calculatedColumnFormula>[39]f0_exc_b0!B2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{75C28E4F-C80D-4ABC-8F6A-8DBD2F364D4A}" name="std.error" dataDxfId="91">
-      <calculatedColumnFormula>[39]f0_exc_b0!C2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{5E6CA2DC-274F-42F5-A8A5-390EFB24C110}" name="2.5% CI" dataDxfId="90">
-      <calculatedColumnFormula>[39]f0_exc_b0!D2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{EAC0DAFE-B91D-4C42-BDC9-4EF8ECE68B5F}" name="97.5% CI" dataDxfId="89">
-      <calculatedColumnFormula>[39]f0_exc_b0!E2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{2CD4C7C7-1CEF-4839-A128-5D2042ACC066}" name="t.value" dataDxfId="88">
-      <calculatedColumnFormula>[39]f0_exc_b0!F2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{4ABD6275-AB55-4007-876B-76D8DB4DFF1F}" name="df" dataDxfId="87">
-      <calculatedColumnFormula>[39]f0_exc_b0!G2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{CE2FF777-20E0-4791-8E86-42CF06A807DA}" name="p.value" dataDxfId="86">
-      <calculatedColumnFormula>[39]f0_exc_b0!H2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{2A298E49-C813-4E10-81DD-DFDD19936088}" name="p.adj." dataDxfId="85">
-      <calculatedColumnFormula>[39]f0_exc_b0!I2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{A6DF8A39-D635-4599-8DD3-BF2C148ED020}" name="signif. " dataDxfId="84">
-      <calculatedColumnFormula>[39]f0_exc_b0!J2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{43307C70-1753-4EDD-A9F4-88C5315A288A}" name="|CI-delta|" dataDxfId="83">
+    <tableColumn id="2" xr3:uid="{352EAC9D-A02A-4CE8-AF89-3ED3FCB5A979}" name="estimate" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{75C28E4F-C80D-4ABC-8F6A-8DBD2F364D4A}" name="std.error" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{5E6CA2DC-274F-42F5-A8A5-390EFB24C110}" name="2.5% CI" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{EAC0DAFE-B91D-4C42-BDC9-4EF8ECE68B5F}" name="97.5% CI" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{2CD4C7C7-1CEF-4839-A128-5D2042ACC066}" name="t.value" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{4ABD6275-AB55-4007-876B-76D8DB4DFF1F}" name="df" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{CE2FF777-20E0-4791-8E86-42CF06A807DA}" name="p.value" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{2A298E49-C813-4E10-81DD-DFDD19936088}" name="p.adj." dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{A6DF8A39-D635-4599-8DD3-BF2C148ED020}" name="signif. " dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{43307C70-1753-4EDD-A9F4-88C5315A288A}" name="|CI-delta|" dataDxfId="48">
       <calculatedColumnFormula>Z3-AB3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18133,22 +17899,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{31E79EDA-219D-4CFA-8AA6-6A991A81B772}" name="Table5" displayName="Table5" ref="A2:K10" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79" totalsRowBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{31E79EDA-219D-4CFA-8AA6-6A991A81B772}" name="Table5" displayName="Table5" ref="A2:K10" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="A2:K10" xr:uid="{31E79EDA-219D-4CFA-8AA6-6A991A81B772}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25702B6E-B402-46EF-BB07-89FAEF761F4F}" name="Predictors" dataDxfId="77">
-      <calculatedColumnFormula>RIGHT([40]l_t_b0!A2,3)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{55B41C0A-72EC-4198-AA0E-BDC398F9A9B6}" name="estimate" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{855FA9D6-FEA4-4049-9614-3F82ACEBC173}" name="std.error" dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{6F9FB966-53EF-492A-8818-43E47D6A804A}" name="2.5% CI" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{79B4821D-DF78-4C65-827E-002BD888F3B1}" name="97.5% CI" dataDxfId="73"/>
-    <tableColumn id="12" xr3:uid="{3558356F-93E9-4BAB-AF09-AF959C11E101}" name="t.value" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{063D2F13-371A-4CFF-9E28-B860ACC5270B}" name="df" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{DF172C73-86B3-4FBF-A011-9108431BAED4}" name="p.value" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{F9DC3D7D-5D08-472E-90A6-84DEB2535DEF}" name="p.adj." dataDxfId="69"/>
-    <tableColumn id="10" xr3:uid="{1FC57EAC-5C7F-4361-B8A1-3963D9B7E878}" name="signif. " dataDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{E2CC2F45-52B6-411C-8857-874E710E7E9B}" name="|CI-delta|" dataDxfId="67">
+    <tableColumn id="1" xr3:uid="{25702B6E-B402-46EF-BB07-89FAEF761F4F}" name="Predictors" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{55B41C0A-72EC-4198-AA0E-BDC398F9A9B6}" name="estimate" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{855FA9D6-FEA4-4049-9614-3F82ACEBC173}" name="std.error" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{6F9FB966-53EF-492A-8818-43E47D6A804A}" name="2.5% CI" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{79B4821D-DF78-4C65-827E-002BD888F3B1}" name="97.5% CI" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{3558356F-93E9-4BAB-AF09-AF959C11E101}" name="t.value" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{063D2F13-371A-4CFF-9E28-B860ACC5270B}" name="df" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{DF172C73-86B3-4FBF-A011-9108431BAED4}" name="p.value" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{F9DC3D7D-5D08-472E-90A6-84DEB2535DEF}" name="p.adj." dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{1FC57EAC-5C7F-4361-B8A1-3963D9B7E878}" name="signif. " dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{E2CC2F45-52B6-411C-8857-874E710E7E9B}" name="|CI-delta|" dataDxfId="32">
       <calculatedColumnFormula>Table5[[#This Row],[estimate]]-Table5[[#This Row],[2.5% CI]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18157,40 +17921,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{873E651E-364D-4C9A-AC67-F669F1DC98F7}" name="Table6" displayName="Table6" ref="A13:K21" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{873E651E-364D-4C9A-AC67-F669F1DC98F7}" name="Table6" displayName="Table6" ref="A13:K21" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A13:K21" xr:uid="{873E651E-364D-4C9A-AC67-F669F1DC98F7}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{13F39383-83C5-45EF-A3DC-AB048CB47D6B}" name="Predictors" dataDxfId="61">
+    <tableColumn id="1" xr3:uid="{13F39383-83C5-45EF-A3DC-AB048CB47D6B}" name="Predictors" dataDxfId="26">
       <calculatedColumnFormula>A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FC01EC59-6FE5-4984-BD8C-56885D9A31B8}" name="estimate" dataDxfId="60">
-      <calculatedColumnFormula>[41]h_t_b0!B2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{497C06E4-D3C0-44F8-972B-B4ED07164CFB}" name="std.error" dataDxfId="59">
-      <calculatedColumnFormula>[41]h_t_b0!C2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{123C5CEC-9EE4-42F1-8816-CAF425B9D6D8}" name="2.5% CI" dataDxfId="58">
-      <calculatedColumnFormula>[41]h_t_b0!D2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{92067161-C954-46A0-8425-5016FA39924E}" name="97.5% CI" dataDxfId="57">
-      <calculatedColumnFormula>[41]h_t_b0!E2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{F9FA392F-0044-4EE9-B9C4-1C335A84554F}" name="t.value" dataDxfId="56">
-      <calculatedColumnFormula>[41]h_t_b0!F2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{2AAB11EB-ED4D-4FE0-AB85-1A33DC205E1E}" name="df" dataDxfId="55">
-      <calculatedColumnFormula>[41]h_t_b0!G2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{D21CE710-DBC3-426C-B448-4B137AF6E93C}" name="p.value" dataDxfId="54">
-      <calculatedColumnFormula>[41]h_t_b0!H2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAA21037-258C-486A-8624-D86C33B3EAD6}" name="p.adj." dataDxfId="53">
-      <calculatedColumnFormula>[41]h_t_b0!I2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{7FD764BF-0FF0-4854-B2D1-69CB096FB29D}" name="signif. " dataDxfId="52">
-      <calculatedColumnFormula>[41]h_t_b0!J2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{017AD943-F50D-4872-8482-F88D6E168424}" name="|CI-delta|" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{FC01EC59-6FE5-4984-BD8C-56885D9A31B8}" name="estimate" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{497C06E4-D3C0-44F8-972B-B4ED07164CFB}" name="std.error" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{123C5CEC-9EE4-42F1-8816-CAF425B9D6D8}" name="2.5% CI" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{92067161-C954-46A0-8425-5016FA39924E}" name="97.5% CI" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{F9FA392F-0044-4EE9-B9C4-1C335A84554F}" name="t.value" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{2AAB11EB-ED4D-4FE0-AB85-1A33DC205E1E}" name="df" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{D21CE710-DBC3-426C-B448-4B137AF6E93C}" name="p.value" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{BAA21037-258C-486A-8624-D86C33B3EAD6}" name="p.adj." dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{7FD764BF-0FF0-4854-B2D1-69CB096FB29D}" name="signif. " dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{017AD943-F50D-4872-8482-F88D6E168424}" name="|CI-delta|" dataDxfId="16">
       <calculatedColumnFormula>B14-D14</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18199,40 +17945,22 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{16906F7D-6662-46E4-84F3-9AAF62C61242}" name="Table7" displayName="Table7" ref="Y13:AI21" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{16906F7D-6662-46E4-84F3-9AAF62C61242}" name="Table7" displayName="Table7" ref="Y13:AI21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="Y13:AI21" xr:uid="{16906F7D-6662-46E4-84F3-9AAF62C61242}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{89F96BA7-E1A0-43BA-9990-4183F8DC6997}" name="Predictors" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{89F96BA7-E1A0-43BA-9990-4183F8DC6997}" name="Predictors" dataDxfId="10">
       <calculatedColumnFormula>A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7CE57966-36A6-4A00-A33D-285D0817534A}" name="estimate" dataDxfId="44">
-      <calculatedColumnFormula>[42]lh_slope_b0!B2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{712F2884-D80C-48C5-9B09-F04127F4ADDE}" name="std.error" dataDxfId="43">
-      <calculatedColumnFormula>[42]lh_slope_b0!C2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{FF4061DC-ECCB-4575-BFAB-736ED74106BB}" name="2.5% CI" dataDxfId="42">
-      <calculatedColumnFormula>[42]lh_slope_b0!D2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{86574847-CC7E-41F3-9B86-76D99ED48F82}" name="97.5% CI" dataDxfId="41">
-      <calculatedColumnFormula>[42]lh_slope_b0!E2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{0D144D85-5573-4622-8DFD-B9F2D6631EE6}" name="t.value" dataDxfId="40">
-      <calculatedColumnFormula>[42]lh_slope_b0!F2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{658C128D-5EF6-4BEA-A291-024002C9B00F}" name="df" dataDxfId="39">
-      <calculatedColumnFormula>[42]lh_slope_b0!G2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{04158CC7-A1BD-4789-8783-0A5E5594F3DE}" name="p.value" dataDxfId="38">
-      <calculatedColumnFormula>[42]lh_slope_b0!H2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{FBA3233F-C3C7-4DA7-A8C9-62499D701BA6}" name="p.adj." dataDxfId="37">
-      <calculatedColumnFormula>[42]lh_slope_b0!I2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{D3824B44-DAFE-4A06-9DCC-51E9B5D08EB3}" name="signif. " dataDxfId="36">
-      <calculatedColumnFormula>[42]lh_slope_b0!J2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{BDAF6820-92C5-4CC2-BE97-6CFF45D70993}" name="|CI-delta|" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{7CE57966-36A6-4A00-A33D-285D0817534A}" name="estimate" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{712F2884-D80C-48C5-9B09-F04127F4ADDE}" name="std.error" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{FF4061DC-ECCB-4575-BFAB-736ED74106BB}" name="2.5% CI" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{86574847-CC7E-41F3-9B86-76D99ED48F82}" name="97.5% CI" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{0D144D85-5573-4622-8DFD-B9F2D6631EE6}" name="t.value" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{658C128D-5EF6-4BEA-A291-024002C9B00F}" name="df" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{04158CC7-A1BD-4789-8783-0A5E5594F3DE}" name="p.value" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FBA3233F-C3C7-4DA7-A8C9-62499D701BA6}" name="p.adj." dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{D3824B44-DAFE-4A06-9DCC-51E9B5D08EB3}" name="signif. " dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{BDAF6820-92C5-4CC2-BE97-6CFF45D70993}" name="|CI-delta|" dataDxfId="0">
       <calculatedColumnFormula>Z14-AB14</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18543,7 +18271,7 @@
   <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="47" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -19125,7 +18853,7 @@
       </c>
       <c r="I5" s="111">
         <f>[5]Mode_f0_exc_b0!I2</f>
-        <v>1.5800000000000001E-7</v>
+        <v>1.68E-7</v>
       </c>
       <c r="J5" s="96" t="str">
         <f>[5]Mode_f0_exc_b0!J2</f>
@@ -19161,7 +18889,7 @@
       </c>
       <c r="R5" s="111">
         <f>[5]Mode_f0_exc_b0!I3</f>
-        <v>2.34E-7</v>
+        <v>2.4699999999999998E-7</v>
       </c>
       <c r="S5" s="91" t="str">
         <f>[5]Mode_f0_exc_b0!J3</f>
@@ -19197,7 +18925,7 @@
       </c>
       <c r="AA5" s="115">
         <f>[5]Mode_f0_exc_b0!I4</f>
-        <v>1.2800000000000001E-7</v>
+        <v>1.36E-7</v>
       </c>
       <c r="AB5" s="91" t="str">
         <f>[5]Mode_f0_exc_b0!J4</f>
@@ -19233,7 +18961,7 @@
       </c>
       <c r="AJ5" s="115">
         <f>[5]Mode_f0_exc_b0!I5</f>
-        <v>1.05E-7</v>
+        <v>1.12E-7</v>
       </c>
       <c r="AK5" s="91" t="str">
         <f>[5]Mode_f0_exc_b0!J5</f>
@@ -20081,7 +19809,7 @@
   <dimension ref="A1:BE10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -20912,7 +20640,7 @@
       </c>
       <c r="I5" s="109">
         <f>[15]Mode_f0_exc_b1!J2</f>
-        <v>0.48899999999999999</v>
+        <v>0.48470000000000002</v>
       </c>
       <c r="J5" s="94">
         <f>[15]Mode_f0_exc_b1!K2</f>
@@ -20948,7 +20676,7 @@
       </c>
       <c r="R5" s="109">
         <f>[15]Mode_f0_exc_b1!J3</f>
-        <v>0.89959999999999996</v>
+        <v>0.89349999999999996</v>
       </c>
       <c r="S5" s="94">
         <f>[15]Mode_f0_exc_b1!K3</f>
@@ -20984,7 +20712,7 @@
       </c>
       <c r="AA5" s="109">
         <f>[15]Mode_f0_exc_b1!J4</f>
-        <v>3.8E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AB5" s="94" t="str">
         <f>[15]Mode_f0_exc_b1!K4</f>
@@ -21020,7 +20748,7 @@
       </c>
       <c r="AJ5" s="109">
         <f>[15]Mode_f0_exc_b1!J5</f>
-        <v>0.76219999999999999</v>
+        <v>0.75649999999999995</v>
       </c>
       <c r="AK5" s="94">
         <f>[15]Mode_f0_exc_b1!K5</f>
@@ -21056,7 +20784,7 @@
       </c>
       <c r="AS5" s="109">
         <f>[15]Mode_f0_exc_b1!J6</f>
-        <v>1.6899999999999998E-2</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="AT5" s="94" t="str">
         <f>[15]Mode_f0_exc_b1!K6</f>
@@ -21092,7 +20820,7 @@
       </c>
       <c r="BB5" s="109">
         <f>[15]Mode_f0_exc_b1!J7</f>
-        <v>4.4299999999999998E-4</v>
+        <v>4.5899999999999999E-4</v>
       </c>
       <c r="BC5" s="94" t="str">
         <f>[15]Mode_f0_exc_b1!K7</f>
@@ -21934,7 +21662,7 @@
       </c>
       <c r="AJ9" s="103">
         <f t="shared" si="19"/>
-        <v>0.76219999999999999</v>
+        <v>0.75649999999999995</v>
       </c>
       <c r="AK9" s="104">
         <f t="shared" si="19"/>
@@ -22259,33 +21987,33 @@
     <mergeCell ref="AL1:AT1"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I10 H7:I8 H3:I5 BA10:BB10 BA7:BB8 BA3:BB5 AR10:AS10 AR7:AS8 AR3:AS5 AI10:AJ10 AI7:AJ8 AI3:AJ5 Z10:AA10 Z7:AA8 Z3:AA5 Q10:R10 Q7:R8 Q3:R5">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC10 BC7:BC8 BC3:BC5 AT3:AT5 AT7:AT8 AT10 AK10 AK7:AK8 AK3:AK5 AB10 AB7:AB8 AB3:AB5 S10 S7:S8 S3:S5 J10 J7:J8 J3:J5">
-    <cfRule type="containsText" dxfId="4" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="132" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="131" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="130" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="129" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
+    <cfRule type="containsText" dxfId="128" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.0001",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22301,8 +22029,8 @@
   </sheetPr>
   <dimension ref="A1:AM29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="47" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="47" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -23812,61 +23540,61 @@
     <mergeCell ref="AL1:AM1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:I5 H7:I8 H10:I10 Q3:R5 Q7:R7 Q10:R10 AI3:AJ5 AI7:AJ8 AI10:AJ10">
-    <cfRule type="cellIs" dxfId="34" priority="14" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="15" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="15" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="17" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J5 J7:J8 J10 S3:S5 S7:S8 S10 AK3:AK5 AK7:AK8 AK10">
-    <cfRule type="containsText" dxfId="22" priority="10" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="123" priority="10" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="11" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="122" priority="11" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="12" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="121" priority="12" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="13" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="120" priority="13" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
+    <cfRule type="containsText" dxfId="119" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.0001",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA5 Z7:AA7 Z10:AA10">
-    <cfRule type="cellIs" dxfId="30" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3:AB5 AB7:AB8 AB10">
-    <cfRule type="containsText" dxfId="26" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="114" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",AB3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="113" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",AB3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="112" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",AB3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="111" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",AB3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23882,8 +23610,8 @@
   </sheetPr>
   <dimension ref="A1:BE10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView showGridLines="0" topLeftCell="AL1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="BD10" sqref="BD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -24444,12 +24172,12 @@
         <v>p&lt;0.01</v>
       </c>
       <c r="BD3" s="70">
-        <f>'B0 PA'!AC4</f>
-        <v>94.087999999999994</v>
+        <f>'B0 PA'!AC3</f>
+        <v>90.968999999999994</v>
       </c>
       <c r="BE3" s="67">
-        <f>'B0 PA'!AM3</f>
-        <v>0.945488879006112</v>
+        <f>'B0 PA'!AD3</f>
+        <v>1.4179999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:57" s="72" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -24673,12 +24401,12 @@
         <v>0</v>
       </c>
       <c r="BD4" s="67">
-        <f>'B0 PA'!AC5</f>
-        <v>8.0340000000000007</v>
+        <f>'B0 PA'!AC4</f>
+        <v>94.087999999999994</v>
       </c>
       <c r="BE4" s="67">
-        <f>'B0 PA'!AM4</f>
-        <v>0.901950415693481</v>
+        <f>'B0 PA'!AD4</f>
+        <v>1.323</v>
       </c>
     </row>
     <row r="5" spans="1:57" s="72" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -24901,13 +24629,13 @@
         <f>[33]PA_f0_exc_b1!K7</f>
         <v>p&lt;0.05</v>
       </c>
-      <c r="BD5" s="78" t="str">
-        <f>'B0 PA'!AC6</f>
-        <v>β0</v>
+      <c r="BD5" s="78">
+        <f>'B0 PA'!AC5</f>
+        <v>8.0340000000000007</v>
       </c>
       <c r="BE5" s="78">
-        <f>'B0 PA'!AM5</f>
-        <v>0.64087133159487397</v>
+        <f>'B0 PA'!AD5</f>
+        <v>0.41799999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:57" s="107" customFormat="1" ht="33.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -26062,33 +25790,33 @@
     <mergeCell ref="AU1:BC1"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I10 H7:I8 H3:I5 BA10:BB10 BA7:BB8 BA3:BB5 AR10:AS10 AR7:AS8 AR3:AS5 AI10:AJ10 AI7:AJ8 AI3:AJ5 Z10:AA10 Z7:AA8 Z3:AA5 Q10:R10 Q7:R8 Q3:R5">
-    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC10 BC7:BC8 BC3:BC5 AT3:AT5 AT7:AT8 AT10 AK10 AK7:AK8 AK3:AK5 AB10 AB7:AB8 AB3:AB5 S10 S7:S8 S3:S5 J10 J7:J8 J3:J5">
-    <cfRule type="containsText" dxfId="13" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
+    <cfRule type="containsText" dxfId="106" priority="2" stopIfTrue="1" operator="containsText" text="p&lt;0.001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.001",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
+    <cfRule type="containsText" dxfId="105" priority="3" stopIfTrue="1" operator="containsText" text="p&lt;0.01">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.01",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
+    <cfRule type="containsText" dxfId="104" priority="4" stopIfTrue="1" operator="containsText" text="p&lt;0.05">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.05",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
+    <cfRule type="containsText" dxfId="103" priority="5" stopIfTrue="1" operator="containsText" text="p&lt;0.1">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.1",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
+    <cfRule type="containsText" dxfId="102" priority="1" stopIfTrue="1" operator="containsText" text="p&lt;0.0001">
       <formula>NOT(ISERROR(SEARCH("p&lt;0.0001",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26101,7 +25829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCED89B-7541-4709-99D1-0E40953C2302}">
   <dimension ref="E5:AB34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26149,9 +25879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA75D8A-458C-4EF4-8CA5-966D1B6FEE89}">
   <dimension ref="A1:BL60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI15" sqref="AI15"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26386,40 +26114,31 @@
         <v>MDC</v>
       </c>
       <c r="N3" s="122">
-        <f>[37]l_f0_b0!B2</f>
         <v>87.427999999999997</v>
       </c>
       <c r="O3" s="123">
-        <f>[37]l_f0_b0!C2</f>
         <v>1.07</v>
       </c>
       <c r="P3" s="123">
-        <f>[37]l_f0_b0!D2</f>
         <v>85.331000000000003</v>
       </c>
       <c r="Q3" s="123">
-        <f>[37]l_f0_b0!E2</f>
         <v>89.525999999999996</v>
       </c>
       <c r="R3" s="179">
-        <f>[37]l_f0_b0!F2</f>
         <v>81.691000000000003</v>
       </c>
       <c r="S3" s="179">
-        <f>[37]l_f0_b0!G2</f>
         <v>10.130000000000001</v>
       </c>
       <c r="T3" s="135">
-        <f>[37]l_f0_b0!H2</f>
         <v>1.2761E-15</v>
       </c>
       <c r="U3" s="135">
-        <f>[37]l_f0_b0!I2</f>
         <v>2.04E-14</v>
       </c>
-      <c r="V3" s="191" t="str">
-        <f>[37]l_f0_b0!J2</f>
-        <v>p&lt;0.001</v>
+      <c r="V3" s="191" t="s">
+        <v>72</v>
       </c>
       <c r="W3" s="176">
         <f t="shared" ref="W3:W10" si="0">N3-P3</f>
@@ -26460,7 +26179,7 @@
       </c>
       <c r="AG3" s="162">
         <f>[5]Mode_f0_exc_b0!I2</f>
-        <v>1.5800000000000001E-7</v>
+        <v>1.68E-7</v>
       </c>
       <c r="AH3" s="202" t="str">
         <f>[5]Mode_f0_exc_b0!J2</f>
@@ -26527,40 +26246,31 @@
         <v>MWH</v>
       </c>
       <c r="N4" s="122">
-        <f>[37]l_f0_b0!B3</f>
         <v>87.581999999999994</v>
       </c>
       <c r="O4" s="123">
-        <f>[37]l_f0_b0!C3</f>
         <v>1.143</v>
       </c>
       <c r="P4" s="123">
-        <f>[37]l_f0_b0!D3</f>
         <v>85.340999999999994</v>
       </c>
       <c r="Q4" s="123">
-        <f>[37]l_f0_b0!E3</f>
         <v>89.822999999999993</v>
       </c>
       <c r="R4" s="179">
-        <f>[37]l_f0_b0!F3</f>
         <v>76.599999999999994</v>
       </c>
       <c r="S4" s="179">
-        <f>[37]l_f0_b0!G3</f>
         <v>11.21</v>
       </c>
       <c r="T4" s="135">
-        <f>[37]l_f0_b0!H3</f>
         <v>1.3445E-16</v>
       </c>
       <c r="U4" s="135">
-        <f>[37]l_f0_b0!I3</f>
         <v>2.1499999999999998E-15</v>
       </c>
-      <c r="V4" s="191" t="str">
-        <f>[37]l_f0_b0!J3</f>
-        <v>p&lt;0.001</v>
+      <c r="V4" s="191" t="s">
+        <v>72</v>
       </c>
       <c r="W4" s="176">
         <f t="shared" si="0"/>
@@ -26601,7 +26311,7 @@
       </c>
       <c r="AG4" s="163">
         <f>[5]Mode_f0_exc_b0!I3</f>
-        <v>2.34E-7</v>
+        <v>2.4699999999999998E-7</v>
       </c>
       <c r="AH4" s="203" t="str">
         <f>[5]Mode_f0_exc_b0!J3</f>
@@ -26669,40 +26379,31 @@
         <v>MYN</v>
       </c>
       <c r="N5" s="122">
-        <f>[37]l_f0_b0!B4</f>
         <v>89.210999999999999</v>
       </c>
       <c r="O5" s="123">
-        <f>[37]l_f0_b0!C4</f>
         <v>1.1830000000000001</v>
       </c>
       <c r="P5" s="123">
-        <f>[37]l_f0_b0!D4</f>
         <v>86.893000000000001</v>
       </c>
       <c r="Q5" s="123">
-        <f>[37]l_f0_b0!E4</f>
         <v>91.53</v>
       </c>
       <c r="R5" s="179">
-        <f>[37]l_f0_b0!F4</f>
         <v>75.412000000000006</v>
       </c>
       <c r="S5" s="179">
-        <f>[37]l_f0_b0!G4</f>
         <v>9.26</v>
       </c>
       <c r="T5" s="135">
-        <f>[37]l_f0_b0!H4</f>
         <v>3.1473E-14</v>
       </c>
       <c r="U5" s="135">
-        <f>[37]l_f0_b0!I4</f>
         <v>5.0399999999999997E-13</v>
       </c>
-      <c r="V5" s="191" t="str">
-        <f>[37]l_f0_b0!J4</f>
-        <v>p&lt;0.001</v>
+      <c r="V5" s="191" t="s">
+        <v>72</v>
       </c>
       <c r="W5" s="176">
         <f t="shared" si="0"/>
@@ -26743,7 +26444,7 @@
       </c>
       <c r="AG5" s="163">
         <f>[5]Mode_f0_exc_b0!I4</f>
-        <v>1.2800000000000001E-7</v>
+        <v>1.36E-7</v>
       </c>
       <c r="AH5" s="203" t="str">
         <f>[5]Mode_f0_exc_b0!J4</f>
@@ -26810,40 +26511,31 @@
         <v>MDQ</v>
       </c>
       <c r="N6" s="126">
-        <f>[37]l_f0_b0!B5</f>
         <v>90.358999999999995</v>
       </c>
       <c r="O6" s="123">
-        <f>[37]l_f0_b0!C5</f>
         <v>1.395</v>
       </c>
       <c r="P6" s="123">
-        <f>[37]l_f0_b0!D5</f>
         <v>87.625</v>
       </c>
       <c r="Q6" s="123">
-        <f>[37]l_f0_b0!E5</f>
         <v>93.093000000000004</v>
       </c>
       <c r="R6" s="179">
-        <f>[37]l_f0_b0!F5</f>
         <v>64.771000000000001</v>
       </c>
       <c r="S6" s="179">
-        <f>[37]l_f0_b0!G5</f>
         <v>10.92</v>
       </c>
       <c r="T6" s="135">
-        <f>[37]l_f0_b0!H5</f>
         <v>1.8184000000000001E-15</v>
       </c>
       <c r="U6" s="135">
-        <f>[37]l_f0_b0!I5</f>
         <v>2.9099999999999997E-14</v>
       </c>
-      <c r="V6" s="191" t="str">
-        <f>[37]l_f0_b0!J5</f>
-        <v>p&lt;0.001</v>
+      <c r="V6" s="191" t="s">
+        <v>72</v>
       </c>
       <c r="W6" s="176">
         <f t="shared" si="0"/>
@@ -26883,7 +26575,7 @@
       </c>
       <c r="AG6" s="164">
         <f>[5]Mode_f0_exc_b0!I5</f>
-        <v>1.05E-7</v>
+        <v>1.12E-7</v>
       </c>
       <c r="AH6" s="204" t="str">
         <f>[5]Mode_f0_exc_b0!J5</f>
@@ -27891,7 +27583,7 @@
         <v>p&lt;0.0001</v>
       </c>
       <c r="AI15" s="176">
-        <f t="shared" ref="AI14:AI21" si="7">Z15-AB15</f>
+        <f t="shared" ref="AI15:AI21" si="7">Z15-AB15</f>
         <v>6.1700254424367564</v>
       </c>
       <c r="AJ15" s="161"/>
@@ -29068,32 +28760,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AF14:AG17 X11:Y11 F11:I11 O11:R11 AF3:AG10 H3:I10 H14:I21 T3:U10 T14:U21 K3:K10 K14:K21 W14:W21 W3:W10">
-    <cfRule type="cellIs" dxfId="136" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF7:AG10">
-    <cfRule type="cellIs" dxfId="135" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H21">
-    <cfRule type="cellIs" dxfId="134" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF18:AG21">
-    <cfRule type="cellIs" dxfId="133" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3:AI10">
-    <cfRule type="cellIs" dxfId="132" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI14:AI21">
-    <cfRule type="cellIs" dxfId="131" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29114,8 +28806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AA7131-6939-4AD7-A411-F3DC957F6760}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>